<commit_message>
Add confirmation modal , CreateAccount page
</commit_message>
<xml_diff>
--- a/public/templates/Concrete.xlsx
+++ b/public/templates/Concrete.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7060"/>
+    <workbookView windowWidth="11590" windowHeight="7240"/>
   </bookViews>
   <sheets>
     <sheet name="Concrete Compressive Strength" sheetId="1" r:id="rId1"/>
@@ -669,8 +669,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1206,13 +1209,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.81818181818182" defaultRowHeight="14.5" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -1241,6 +1244,35 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>540</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>162</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1040</v>
+      </c>
+      <c r="G2" s="1">
+        <v>676</v>
+      </c>
+      <c r="H2" s="1">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1">
+        <v>79.98611076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>